<commit_message>
feat: sending updated xlsx file with the kodebarang is uuid
</commit_message>
<xml_diff>
--- a/public/samples/sample_barang.xlsx
+++ b/public/samples/sample_barang.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\inventara\public\samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\IAe-TC-web\public\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{476E698F-D9D3-4B8E-9F53-78271E76E119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4144211C-690A-48EF-95ED-2A5F18E3A138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6594B437-2A68-4CB4-B114-1C939C4CC6CB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{6594B437-2A68-4CB4-B114-1C939C4CC6CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,69 +25,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+  <si>
+    <t>nama_barang</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>kondisi</t>
+  </si>
+  <si>
+    <t>garansi</t>
+  </si>
+  <si>
+    <t>ruangan</t>
+  </si>
+  <si>
+    <t>photo</t>
+  </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <t>Dipinjam</t>
+  </si>
+  <si>
+    <t>Bagus</t>
+  </si>
+  <si>
+    <t>Aktiva 10112</t>
+  </si>
+  <si>
+    <t>Proyektor</t>
+  </si>
+  <si>
+    <t>Tidak Dipinjam</t>
+  </si>
+  <si>
+    <t>Kurang Bagus</t>
+  </si>
+  <si>
+    <t>Aktiva 2999</t>
+  </si>
+  <si>
+    <t>Komputer</t>
+  </si>
+  <si>
+    <t>Rusak</t>
+  </si>
+  <si>
+    <t>Aktiva 6557</t>
+  </si>
   <si>
     <t>kode_barang</t>
-  </si>
-  <si>
-    <t>nama_barang</t>
-  </si>
-  <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>kondisi</t>
-  </si>
-  <si>
-    <t>garansi</t>
-  </si>
-  <si>
-    <t>ruangan</t>
-  </si>
-  <si>
-    <t>photo</t>
-  </si>
-  <si>
-    <t>HP</t>
-  </si>
-  <si>
-    <t>Aktiva 8888</t>
-  </si>
-  <si>
-    <t>Dipinjam</t>
-  </si>
-  <si>
-    <t>Bagus</t>
-  </si>
-  <si>
-    <t>Aktiva 10112</t>
-  </si>
-  <si>
-    <t>Proyektor</t>
-  </si>
-  <si>
-    <t>Aktiva 5665</t>
-  </si>
-  <si>
-    <t>Tidak Dipinjam</t>
-  </si>
-  <si>
-    <t>Kurang Bagus</t>
-  </si>
-  <si>
-    <t>Aktiva 2999</t>
-  </si>
-  <si>
-    <t>Komputer</t>
-  </si>
-  <si>
-    <t>Aktiva 6656</t>
-  </si>
-  <si>
-    <t>Rusak</t>
-  </si>
-  <si>
-    <t>Aktiva 6557</t>
   </si>
 </sst>
 </file>
@@ -325,9 +316,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -365,7 +356,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -471,7 +462,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -613,7 +604,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -624,13 +615,12 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="1" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" customWidth="1"/>
@@ -641,87 +631,81 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="E2" s="2">
         <v>44969</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="E3" s="2">
         <v>43902</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>18</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E4" s="2">
         <v>48977</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G4" s="1"/>
     </row>

</xml_diff>